<commit_message>
final fix for data
</commit_message>
<xml_diff>
--- a/datasets/Date_Fruit_Datasets.xlsx
+++ b/datasets/Date_Fruit_Datasets.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\AAAAAAAAAAMAGISTER\Semestr2\UMA\uma-projekt\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67092410-F3F9-45A2-9A26-535DB90EC80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDEB20B-7CF0-4916-B526-D4371646EB00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,9 +17,6 @@
     <sheet name="Citation_Request" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
-  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="25">
   <si>
     <t>AREA</t>
   </si>
@@ -147,18 +144,6 @@
 https://www.hindawi.com/journals/mpe/2021/4793293/</t>
     </r>
   </si>
-  <si>
-    <t>Row Labels</t>
-  </si>
-  <si>
-    <t>(blank)</t>
-  </si>
-  <si>
-    <t>Grand Total</t>
-  </si>
-  <si>
-    <t>Count of Class</t>
-  </si>
 </sst>
 </file>
 
@@ -245,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -259,10 +244,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -279,2803 +260,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Marcin" refreshedDate="45264.014752777781" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="899" xr:uid="{2FBB3B3D-C00A-45EE-BB3B-D0DBE3E8DB6A}">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="Q1:Q1048576" sheet="Date_Fruit_Datasets"/>
-  </cacheSource>
-  <cacheFields count="1">
-    <cacheField name="Class" numFmtId="0">
-      <sharedItems containsBlank="1" count="8">
-        <s v="BERHI"/>
-        <s v="DEGLET"/>
-        <s v="DOKOL"/>
-        <s v="IRAQI"/>
-        <s v="ROTANA"/>
-        <s v="SAFAVI"/>
-        <s v="SOGAY"/>
-        <m/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="899">
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="7"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{30D70888-75DD-47A3-82C6-9DC74ADAE9D2}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="R1:S10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="1">
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="9">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Class" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3343,9 +527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T899"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="W17" sqref="W17"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3418,12 +600,8 @@
       <c r="Q1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="S1" t="s">
-        <v>28</v>
-      </c>
+      <c r="R1"/>
+      <c r="S1"/>
       <c r="T1"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -3478,12 +656,6 @@
       <c r="Q2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="R2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="S2">
-        <v>65</v>
-      </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -3537,12 +709,6 @@
       <c r="Q3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="R3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="S3">
-        <v>98</v>
-      </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
@@ -3596,12 +762,6 @@
       <c r="Q4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="R4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="S4">
-        <v>204</v>
-      </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -3655,12 +815,6 @@
       <c r="Q5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="R5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="S5">
-        <v>72</v>
-      </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
@@ -3714,12 +868,6 @@
       <c r="Q6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="R6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="S6">
-        <v>166</v>
-      </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
@@ -3773,12 +921,6 @@
       <c r="Q7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="R7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="S7">
-        <v>199</v>
-      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
@@ -3832,12 +974,6 @@
       <c r="Q8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="R8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="S8">
-        <v>94</v>
-      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
@@ -3891,9 +1027,6 @@
       <c r="Q9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="R9" s="7" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
@@ -3947,12 +1080,6 @@
       <c r="Q10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="R10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="S10">
-        <v>898</v>
-      </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -51073,7 +48200,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>